<commit_message>
Can make weather demo queue
</commit_message>
<xml_diff>
--- a/P2_Dispatcher/WeatherDemoInput.xlsx
+++ b/P2_Dispatcher/WeatherDemoInput.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\GetawayGurus\P2_Performer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\GetawayGurus\P2_Dispatcher\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49159186-2A55-44FE-87A7-B2B0009731A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD3012D5-2FD8-4798-850C-DCF43FFE4A30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3020" yWindow="1320" windowWidth="17300" windowHeight="9980" xr2:uid="{24A87DED-BB21-43B2-AFBB-3F918952F845}"/>
+    <workbookView xWindow="3180" yWindow="2820" windowWidth="17300" windowHeight="9980" xr2:uid="{24A87DED-BB21-43B2-AFBB-3F918952F845}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -72,6 +72,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="mm/dd/yyyy"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -103,7 +106,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -421,7 +424,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C2" sqref="C2:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -490,5 +493,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>